<commit_message>
20251122 Estable previa prueba checkboxes
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS WEB\CENTRO POLICIAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CENTRO POLICIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66F9774C-9AEF-4207-B98F-78A07C51A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1707B57E-E638-46D5-9523-BAB8A0F7AC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{D5B539C2-7882-4F63-8F95-63521C8537F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5B539C2-7882-4F63-8F95-63521C8537F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>DICCIONARIO CAMPOS CENTRO POLICIAL</t>
   </si>
@@ -108,6 +97,15 @@
   </si>
   <si>
     <t>200: IDENTIFICACIÓN</t>
+  </si>
+  <si>
+    <t>fecha_DerAlc</t>
+  </si>
+  <si>
+    <t>hora_DerAlc</t>
+  </si>
+  <si>
+    <t>201:DERECHOS DE ALCOHOLEMIA</t>
   </si>
 </sst>
 </file>
@@ -514,27 +512,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560D72AC-9304-42CD-8A76-E2285C8AADBA}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.90625" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
-    <col min="3" max="3" width="52.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -545,7 +543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -553,7 +551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -561,7 +559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -569,7 +567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -577,7 +575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -585,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -593,7 +591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -601,7 +599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -609,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -617,7 +615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -625,7 +623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -633,7 +631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -641,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -649,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -657,7 +655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -665,7 +663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -673,7 +671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -681,12 +679,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>